<commit_message>
updated stakeholder needs table
</commit_message>
<xml_diff>
--- a/2_Analyse/2_Stakeholder-Tabelle_Erfordernisse.xlsx
+++ b/2_Analyse/2_Stakeholder-Tabelle_Erfordernisse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alenn\OneDrive\Dokumente\Studium\Abschlussprojekt\2_Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Assistenz_Dienstplaner\GitHub_Repository\2_Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A60EB1E-727E-4EEA-A3E5-B7EB09F26299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F65F6C-8EFD-4FF3-85BA-36FA015C2E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A85476F-D9C6-4364-AF75-1C49FB25F5D3}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8A85476F-D9C6-4364-AF75-1C49FB25F5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,12 +378,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -427,6 +421,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -435,12 +432,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -778,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF15D57-CCDA-4C54-BF8C-B7476BD37DF6}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,10 +796,10 @@
       <c r="D1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="11"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -821,47 +812,47 @@
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+    <row r="5" spans="1:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="13" t="s">
         <v>85</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -869,23 +860,23 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="14" t="s">
+      <c r="A7" s="11"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="10" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13" t="s">
+      <c r="A8" s="11"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="10" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="216" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
@@ -900,7 +891,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
@@ -915,7 +906,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
@@ -930,7 +921,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
@@ -945,7 +936,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
@@ -960,7 +951,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
@@ -975,7 +966,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="3" t="s">
         <v>42</v>
       </c>
@@ -990,7 +981,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
@@ -1005,13 +996,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
+      <c r="A17" s="11"/>
       <c r="E17" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1025,7 +1016,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
@@ -1037,7 +1028,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
@@ -1049,7 +1040,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
@@ -1061,7 +1052,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="5" t="s">
         <v>11</v>
       </c>
@@ -1076,7 +1067,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
@@ -1091,10 +1082,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
+      <c r="A24" s="11"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
+      <c r="A25" s="11"/>
       <c r="E25" s="9" t="s">
         <v>77</v>
       </c>
@@ -1122,7 +1113,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="11" t="s">
         <v>71</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -1139,7 +1130,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="3" t="s">
         <v>19</v>
       </c>
@@ -1151,7 +1142,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
@@ -1166,7 +1157,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
@@ -1178,7 +1169,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="3" t="s">
         <v>15</v>
       </c>
@@ -1193,7 +1184,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="3" t="s">
         <v>42</v>
       </c>
@@ -1205,10 +1196,10 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
+      <c r="A34" s="11"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
+      <c r="A35" s="11"/>
     </row>
     <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">

</xml_diff>

<commit_message>
small changes on stakeholder requirements
</commit_message>
<xml_diff>
--- a/2_Analyse/2_Stakeholder-Tabelle_Erfordernisse.xlsx
+++ b/2_Analyse/2_Stakeholder-Tabelle_Erfordernisse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Assistenz_Dienstplaner\GitHub_Repository\2_Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F65F6C-8EFD-4FF3-85BA-36FA015C2E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EA3AAE-FF44-4418-943A-AA868FC96FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8A85476F-D9C6-4364-AF75-1C49FB25F5D3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A85476F-D9C6-4364-AF75-1C49FB25F5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -277,9 +277,6 @@
 …die persönlichen Wünsche der Assistent*innen bezüglich der Einsatzzeiten verfügbar haben, um diese nach Möglichkeit in der Dienstplanung berücksichtigen zu können.</t>
   </si>
   <si>
-    <t>Beratungsstellen für die Persönliche Assistent müssen ihre Kund*innen umfassend informieren und beraten können.</t>
-  </si>
-  <si>
     <t>Die Schichten in beiden Teams müssen koordiniert werden.</t>
   </si>
   <si>
@@ -317,9 +314,6 @@
     <t>…Möglichkeiten zur Genehmigung oder Ablehnung von Wünschen und Änderungsanfragen der Assistent*innen verfügbar haben, um die Assistenz gemäß der eigenen Bedürfnisse gestalten zu können.</t>
   </si>
   <si>
-    <t>...sowohl Möglichkeiten zur Vorab-Genehmigung als auch Genehmigung auf Anfrage verfügbar haben, um den Umgang mit Anfragen der Assistent*innen effektiv gestalten zu können.</t>
-  </si>
-  <si>
     <t>…um die verbleibenden Tage bis zur Dienstplanung wissen, um Assistent*innen, die ihre Verfügbarkeiten noch nicht eingereicht haben, rechtzeitig zu erinnern.</t>
   </si>
   <si>
@@ -339,6 +333,12 @@
   </si>
   <si>
     <t>Beratungsstellen</t>
+  </si>
+  <si>
+    <t>Lohnbüros benötigen eine Dokumentation der geleisteten Arbeitszeit der Assistent*innen</t>
+  </si>
+  <si>
+    <t>Beratungsstellen für die Persönliche Assistent wollen umfassend informieren und beraten können.</t>
   </si>
 </sst>
 </file>
@@ -770,7 +770,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,7 +825,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -833,16 +833,13 @@
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
-      <c r="E5" s="8" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
@@ -850,13 +847,13 @@
         <v>19</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>85</v>
-      </c>
       <c r="E6" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -864,7 +861,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -872,7 +869,7 @@
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="216" x14ac:dyDescent="0.3">
@@ -929,10 +926,10 @@
         <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -959,7 +956,7 @@
         <v>17</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>73</v>
@@ -1063,7 +1060,7 @@
         <v>41</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1072,13 +1069,13 @@
         <v>19</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1087,7 +1084,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="E25" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1101,10 +1098,10 @@
         <v>21</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1228,7 +1225,7 @@
         <v>19</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>49</v>
@@ -1248,9 +1245,14 @@
         <v>48</v>
       </c>
     </row>
+    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D44" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="46" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>19</v>
@@ -1259,7 +1261,7 @@
         <v>50</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>